<commit_message>
task 2 added info
</commit_message>
<xml_diff>
--- a/task2/parameterChanges.xlsx
+++ b/task2/parameterChanges.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saram\OneDrive\COURSES\Modeling and Simulation\project\modsim\influenza1\task2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/066c60c930f0ee7e/COURSES/Modeling and Simulation/project/modsim/influenza1/task2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40350DF0-1073-400B-B0F8-F05FA398D344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="2610" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14505" yWindow="2610" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>